<commit_message>
Well Completion Version A depth field from int to float
</commit_message>
<xml_diff>
--- a/src/ogrre_data_cleaning/processor_schemas/ISGS Well Completion Schema.xlsx
+++ b/src/ogrre_data_cleaning/processor_schemas/ISGS Well Completion Schema.xlsx
@@ -40,7 +40,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId22" roundtripDataChecksum="HXuYbnKHqAD0RcUQGJQzBmneLNv162D2x+0enRyAz7c="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId22" roundtripDataChecksum="EqKHIqwbW4dnPEobRb/Q5DiwreC5AjybFd1OClSNG8c="/>
     </ext>
   </extLst>
 </workbook>
@@ -3936,7 +3936,7 @@
     <xdr:ext cx="2028825" cy="2762250"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="There are 4 minor variations of this format" id="0" name="image8.png" title="Completion_A"/>
+        <xdr:cNvPr descr="There are 4 minor variations of this format" id="0" name="image5.png" title="Completion_A"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3964,7 +3964,7 @@
     <xdr:ext cx="2009775" cy="2771775"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Completion_C Page 1"/>
+        <xdr:cNvPr id="0" name="image7.png" title="Completion_C Page 1"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3992,7 +3992,7 @@
     <xdr:ext cx="2000250" cy="2752725"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Completion_C Page 2"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Completion_C Page 2"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4020,7 +4020,7 @@
     <xdr:ext cx="1981200" cy="2705100"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="There are two minor variations of this format" id="0" name="image2.png" title="Competion_D Page 1"/>
+        <xdr:cNvPr descr="There are two minor variations of this format" id="0" name="image8.png" title="Competion_D Page 1"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4048,7 +4048,7 @@
     <xdr:ext cx="1990725" cy="2705100"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="There are two variations of this format" id="0" name="image4.png" title="Completion_D Page 2"/>
+        <xdr:cNvPr descr="There are two variations of this format" id="0" name="image3.png" title="Completion_D Page 2"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4076,7 +4076,7 @@
     <xdr:ext cx="2047875" cy="2781300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Completion_E Page 1"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Completion_E Page 1"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4104,7 +4104,7 @@
     <xdr:ext cx="1952625" cy="2781300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Completion_E"/>
+        <xdr:cNvPr id="0" name="image9.png" title="Completion_E"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4132,7 +4132,7 @@
     <xdr:ext cx="1762125" cy="2324100"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4160,7 +4160,7 @@
     <xdr:ext cx="2581275" cy="2133600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -34981,9 +34981,6 @@
       <c r="D37" s="15">
         <v>0.903</v>
       </c>
-      <c r="E37" s="14" t="s">
-        <v>89</v>
-      </c>
       <c r="F37" s="14">
         <v>139.0</v>
       </c>
@@ -35014,9 +35011,11 @@
         <v>99</v>
       </c>
       <c r="D38" s="18">
-        <v>0.827</v>
-      </c>
-      <c r="E38" s="13"/>
+        <v>0.94</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>89</v>
+      </c>
       <c r="F38" s="11">
         <v>139.0</v>
       </c>
@@ -43127,7 +43126,7 @@
         <v>0.876</v>
       </c>
       <c r="T3" s="25">
-        <v>0.541</v>
+        <v>0.945</v>
       </c>
     </row>
     <row r="4">
@@ -43183,7 +43182,7 @@
         <v>0.841</v>
       </c>
       <c r="T4" s="21">
-        <v>0.64</v>
+        <v>0.958</v>
       </c>
     </row>
     <row r="5">
@@ -43351,7 +43350,7 @@
         <v>0.949</v>
       </c>
       <c r="T7" s="25">
-        <v>0.583</v>
+        <v>0.971</v>
       </c>
     </row>
     <row r="8">
@@ -43407,7 +43406,7 @@
         <v>0.947</v>
       </c>
       <c r="T8" s="21">
-        <v>0.442</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="9">
@@ -43759,7 +43758,7 @@
         <v>0.982</v>
       </c>
       <c r="T15" s="25">
-        <v>0.982</v>
+        <v>0.978</v>
       </c>
     </row>
     <row r="16">
@@ -44075,7 +44074,7 @@
         <v>0.964</v>
       </c>
       <c r="T21" s="25">
-        <v>0.927</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="22">
@@ -44131,7 +44130,7 @@
         <v>0.971</v>
       </c>
       <c r="T22" s="21">
-        <v>0.977</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="23">
@@ -44187,7 +44186,7 @@
         <v>0.982</v>
       </c>
       <c r="T23" s="25">
-        <v>0.986</v>
+        <v>0.991</v>
       </c>
     </row>
     <row r="24">
@@ -44213,8 +44212,8 @@
       <c r="H24" s="31" t="s">
         <v>436</v>
       </c>
-      <c r="I24" s="31" t="s">
-        <v>437</v>
+      <c r="I24" s="21" t="s">
+        <v>260</v>
       </c>
       <c r="J24" s="31"/>
       <c r="K24" s="31"/>
@@ -44267,8 +44266,8 @@
       <c r="H25" s="32" t="s">
         <v>436</v>
       </c>
-      <c r="I25" s="32" t="s">
-        <v>437</v>
+      <c r="I25" s="25" t="s">
+        <v>260</v>
       </c>
       <c r="J25" s="32"/>
       <c r="K25" s="32"/>
@@ -44639,7 +44638,7 @@
         <v>0.986</v>
       </c>
       <c r="T32" s="21">
-        <v>0.995</v>
+        <v>0.991</v>
       </c>
     </row>
     <row r="33">
@@ -44695,7 +44694,7 @@
         <v>0.717</v>
       </c>
       <c r="T33" s="25">
-        <v>0.66</v>
+        <v>0.822</v>
       </c>
     </row>
     <row r="34">
@@ -44751,7 +44750,7 @@
         <v>0.853</v>
       </c>
       <c r="T34" s="21">
-        <v>0.648</v>
+        <v>0.881</v>
       </c>
     </row>
     <row r="35">
@@ -44807,7 +44806,7 @@
         <v>0.989</v>
       </c>
       <c r="T35" s="25">
-        <v>0.984</v>
+        <v>0.979</v>
       </c>
     </row>
     <row r="36">
@@ -44917,7 +44916,7 @@
         <v>0.889</v>
       </c>
       <c r="T37" s="25">
-        <v>0.286</v>
+        <v>0.928</v>
       </c>
     </row>
     <row r="38">
@@ -44973,7 +44972,7 @@
         <v>0.949</v>
       </c>
       <c r="T38" s="21">
-        <v>0.571</v>
+        <v>0.981</v>
       </c>
     </row>
     <row r="39">
@@ -45029,7 +45028,7 @@
         <v>0.814</v>
       </c>
       <c r="T39" s="25">
-        <v>0.427</v>
+        <v>0.942</v>
       </c>
     </row>
     <row r="40">
@@ -45085,7 +45084,7 @@
         <v>0.671</v>
       </c>
       <c r="T40" s="21">
-        <v>0.507</v>
+        <v>0.939</v>
       </c>
     </row>
     <row r="41">
@@ -45253,7 +45252,7 @@
         <v>0.89</v>
       </c>
       <c r="T43" s="25">
-        <v>0.467</v>
+        <v>0.959</v>
       </c>
     </row>
     <row r="44">
@@ -45309,7 +45308,7 @@
         <v>0.731</v>
       </c>
       <c r="T44" s="21">
-        <v>0.542</v>
+        <v>0.909</v>
       </c>
     </row>
     <row r="45">
@@ -45389,8 +45388,8 @@
       <c r="H46" s="31" t="s">
         <v>436</v>
       </c>
-      <c r="I46" s="31" t="s">
-        <v>437</v>
+      <c r="I46" s="21" t="s">
+        <v>260</v>
       </c>
       <c r="J46" s="31"/>
       <c r="K46" s="31"/>
@@ -45589,8 +45588,8 @@
       <c r="H50" s="31" t="s">
         <v>436</v>
       </c>
-      <c r="I50" s="31" t="s">
-        <v>437</v>
+      <c r="I50" s="21" t="s">
+        <v>260</v>
       </c>
       <c r="J50" s="31"/>
       <c r="K50" s="31"/>
@@ -45763,8 +45762,8 @@
       <c r="H54" s="31" t="s">
         <v>436</v>
       </c>
-      <c r="I54" s="31" t="s">
-        <v>437</v>
+      <c r="I54" s="21" t="s">
+        <v>260</v>
       </c>
       <c r="J54" s="31"/>
       <c r="K54" s="31"/>
@@ -45963,8 +45962,8 @@
       <c r="H58" s="31" t="s">
         <v>436</v>
       </c>
-      <c r="I58" s="31" t="s">
-        <v>437</v>
+      <c r="I58" s="21" t="s">
+        <v>260</v>
       </c>
       <c r="J58" s="31"/>
       <c r="K58" s="31"/>
@@ -46163,7 +46162,7 @@
         <v>0.97</v>
       </c>
       <c r="T62" s="21">
-        <v>0.985</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="63">
@@ -46319,7 +46318,7 @@
         <v>0.931</v>
       </c>
       <c r="T65" s="25">
-        <v>0.952</v>
+        <v>0.984</v>
       </c>
     </row>
     <row r="66">
@@ -46417,7 +46416,7 @@
         <v>0.833</v>
       </c>
       <c r="T67" s="25">
-        <v>0.857</v>
+        <v>0.963</v>
       </c>
     </row>
     <row r="68">
@@ -46471,7 +46470,7 @@
         <v>0.863</v>
       </c>
       <c r="T68" s="21">
-        <v>0.792</v>
+        <v>0.849</v>
       </c>
     </row>
     <row r="69">
@@ -46637,7 +46636,7 @@
         <v>0.558</v>
       </c>
       <c r="T71" s="25">
-        <v>0.733</v>
+        <v>0.769</v>
       </c>
     </row>
     <row r="72">
@@ -46691,7 +46690,7 @@
         <v>0.718</v>
       </c>
       <c r="T72" s="21">
-        <v>0.68</v>
+        <v>0.782</v>
       </c>
     </row>
     <row r="73">
@@ -46895,7 +46894,7 @@
         <v>0.771</v>
       </c>
       <c r="T76" s="21">
-        <v>0.774</v>
+        <v>0.851</v>
       </c>
     </row>
     <row r="77">
@@ -46949,7 +46948,7 @@
         <v>0.971</v>
       </c>
       <c r="T77" s="25">
-        <v>0.981</v>
+        <v>0.995</v>
       </c>
     </row>
     <row r="78">
@@ -46998,6 +46997,7 @@
   <autoFilter ref="$A$1:$T$77">
     <sortState ref="A1:T77">
       <sortCondition ref="C1:C77"/>
+      <sortCondition ref="D1:D77"/>
     </sortState>
   </autoFilter>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update ISGS Well Completion Schema.xlsx
</commit_message>
<xml_diff>
--- a/src/ogrre_data_cleaning/processor_schemas/ISGS Well Completion Schema.xlsx
+++ b/src/ogrre_data_cleaning/processor_schemas/ISGS Well Completion Schema.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6502" uniqueCount="872">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6502" uniqueCount="871">
   <si>
     <t>Naming Scheme as of 6/17/2024</t>
   </si>
@@ -2171,9 +2171,6 @@
   </si>
   <si>
     <t>Operator_Signature_Date</t>
-  </si>
-  <si>
-    <t>string_to_date</t>
   </si>
   <si>
     <t>Well_Inspector</t>
@@ -3989,7 +3986,7 @@
     <xdr:ext cx="2028825" cy="2762250"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="There are 4 minor variations of this format" id="0" name="image8.png" title="Completion_A"/>
+        <xdr:cNvPr descr="There are 4 minor variations of this format" id="0" name="image6.png" title="Completion_A"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4017,7 +4014,7 @@
     <xdr:ext cx="2009775" cy="2771775"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Completion_C Page 1"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Completion_C Page 1"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4045,7 +4042,7 @@
     <xdr:ext cx="2000250" cy="2752725"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Completion_C Page 2"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Completion_C Page 2"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4073,7 +4070,7 @@
     <xdr:ext cx="1981200" cy="2705100"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="There are two minor variations of this format" id="0" name="image3.png" title="Competion_D Page 1"/>
+        <xdr:cNvPr descr="There are two minor variations of this format" id="0" name="image7.png" title="Competion_D Page 1"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4129,7 +4126,7 @@
     <xdr:ext cx="2047875" cy="2781300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Completion_E Page 1"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Completion_E Page 1"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4157,7 +4154,7 @@
     <xdr:ext cx="1952625" cy="2781300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.png" title="Completion_E"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Completion_E"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4185,7 +4182,7 @@
     <xdr:ext cx="1762125" cy="2324100"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4213,7 +4210,7 @@
     <xdr:ext cx="2581275" cy="2133600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -19350,7 +19347,7 @@
         <v>270</v>
       </c>
       <c r="I61" s="30" t="s">
-        <v>708</v>
+        <v>271</v>
       </c>
       <c r="J61" s="39"/>
       <c r="K61" s="39"/>
@@ -19401,7 +19398,7 @@
         <v>62.0</v>
       </c>
       <c r="D62" s="38" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="E62" s="38" t="s">
         <v>258</v>
@@ -19463,7 +19460,7 @@
         <v>63.0</v>
       </c>
       <c r="D63" s="39" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E63" s="39" t="s">
         <v>269</v>
@@ -19531,7 +19528,7 @@
         <v>64.0</v>
       </c>
       <c r="D64" s="38" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E64" s="38" t="s">
         <v>258</v>
@@ -19573,7 +19570,7 @@
         <v>65.0</v>
       </c>
       <c r="D65" s="39" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E65" s="39" t="s">
         <v>258</v>
@@ -19586,7 +19583,7 @@
         <v>270</v>
       </c>
       <c r="I65" s="30" t="s">
-        <v>708</v>
+        <v>271</v>
       </c>
       <c r="J65" s="39"/>
       <c r="K65" s="39"/>
@@ -19617,7 +19614,7 @@
         <v>66.0</v>
       </c>
       <c r="D66" s="38" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="E66" s="38" t="s">
         <v>269</v>
@@ -19679,7 +19676,7 @@
         <v>67.0</v>
       </c>
       <c r="D67" s="39" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E67" s="39" t="s">
         <v>258</v>
@@ -19741,7 +19738,7 @@
         <v>68.0</v>
       </c>
       <c r="D68" s="38" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E68" s="38" t="s">
         <v>269</v>
@@ -19964,10 +19961,10 @@
         <v>438</v>
       </c>
       <c r="T1" s="44" t="s">
+        <v>715</v>
+      </c>
+      <c r="U1" s="44" t="s">
         <v>716</v>
-      </c>
-      <c r="U1" s="44" t="s">
-        <v>717</v>
       </c>
       <c r="V1" s="44" t="s">
         <v>435</v>
@@ -19978,13 +19975,13 @@
         <v>44</v>
       </c>
       <c r="B2" s="38" t="s">
+        <v>717</v>
+      </c>
+      <c r="C2" s="38">
+        <v>1.0</v>
+      </c>
+      <c r="D2" s="38" t="s">
         <v>718</v>
-      </c>
-      <c r="C2" s="38">
-        <v>1.0</v>
-      </c>
-      <c r="D2" s="38" t="s">
-        <v>719</v>
       </c>
       <c r="E2" s="38" t="s">
         <v>258</v>
@@ -20036,13 +20033,13 @@
         <v>44</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C3" s="39">
         <v>2.0</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="E3" s="39" t="s">
         <v>258</v>
@@ -20094,13 +20091,13 @@
         <v>44</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C4" s="38">
         <v>3.0</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E4" s="38" t="s">
         <v>258</v>
@@ -20152,13 +20149,13 @@
         <v>44</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C5" s="39">
         <v>4.0</v>
       </c>
       <c r="D5" s="39" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E5" s="39" t="s">
         <v>258</v>
@@ -20210,7 +20207,7 @@
         <v>44</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C6" s="38">
         <v>5.0</v>
@@ -20268,13 +20265,13 @@
         <v>44</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C7" s="39">
         <v>6.0</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E7" s="39" t="s">
         <v>258</v>
@@ -20328,13 +20325,13 @@
         <v>44</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C8" s="38">
         <v>7.0</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E8" s="38" t="s">
         <v>258</v>
@@ -20388,13 +20385,13 @@
         <v>44</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C9" s="39">
         <v>8.0</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E9" s="39" t="s">
         <v>258</v>
@@ -20448,13 +20445,13 @@
         <v>44</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C10" s="38">
         <v>9.0</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="E10" s="38" t="s">
         <v>258</v>
@@ -20508,13 +20505,13 @@
         <v>44</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C11" s="39">
         <v>10.0</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E11" s="39" t="s">
         <v>258</v>
@@ -20566,7 +20563,7 @@
         <v>44</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C12" s="38">
         <v>11.0</v>
@@ -20624,7 +20621,7 @@
         <v>44</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C13" s="39">
         <v>12.0</v>
@@ -20682,7 +20679,7 @@
         <v>44</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C14" s="38">
         <v>13.0</v>
@@ -20732,7 +20729,7 @@
         <v>44</v>
       </c>
       <c r="B15" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C15" s="39">
         <v>14.0</v>
@@ -20792,7 +20789,7 @@
         <v>44</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C16" s="38">
         <v>15.0</v>
@@ -20850,7 +20847,7 @@
         <v>44</v>
       </c>
       <c r="B17" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C17" s="39">
         <v>16.0</v>
@@ -20908,13 +20905,13 @@
         <v>44</v>
       </c>
       <c r="B18" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C18" s="38">
         <v>17.0</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="E18" s="38" t="s">
         <v>258</v>
@@ -20966,7 +20963,7 @@
         <v>44</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C19" s="39">
         <v>18.0</v>
@@ -21024,13 +21021,13 @@
         <v>44</v>
       </c>
       <c r="B20" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C20" s="38">
         <v>19.0</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E20" s="38" t="s">
         <v>258</v>
@@ -21064,7 +21061,7 @@
         <v>44</v>
       </c>
       <c r="B21" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C21" s="39">
         <v>20.0</v>
@@ -21124,7 +21121,7 @@
         <v>44</v>
       </c>
       <c r="B22" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C22" s="38">
         <v>21.0</v>
@@ -21184,13 +21181,13 @@
         <v>44</v>
       </c>
       <c r="B23" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C23" s="39">
         <v>22.0</v>
       </c>
       <c r="D23" s="39" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="E23" s="39" t="s">
         <v>258</v>
@@ -21242,13 +21239,13 @@
         <v>44</v>
       </c>
       <c r="B24" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C24" s="38">
         <v>23.0</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="E24" s="38" t="s">
         <v>258</v>
@@ -21261,7 +21258,7 @@
         <v>270</v>
       </c>
       <c r="I24" s="26" t="s">
-        <v>708</v>
+        <v>271</v>
       </c>
       <c r="J24" s="38"/>
       <c r="K24" s="38"/>
@@ -21302,7 +21299,7 @@
         <v>44</v>
       </c>
       <c r="B25" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C25" s="39">
         <v>24.0</v>
@@ -21362,13 +21359,13 @@
         <v>44</v>
       </c>
       <c r="B26" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C26" s="38">
         <v>25.0</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E26" s="38" t="s">
         <v>258</v>
@@ -21420,7 +21417,7 @@
         <v>44</v>
       </c>
       <c r="B27" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C27" s="39">
         <v>26.0</v>
@@ -21439,7 +21436,7 @@
         <v>270</v>
       </c>
       <c r="I27" s="30" t="s">
-        <v>708</v>
+        <v>271</v>
       </c>
       <c r="J27" s="39"/>
       <c r="K27" s="39"/>
@@ -21480,13 +21477,13 @@
         <v>44</v>
       </c>
       <c r="B28" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C28" s="38">
         <v>27.0</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E28" s="38" t="s">
         <v>258</v>
@@ -21499,7 +21496,7 @@
         <v>270</v>
       </c>
       <c r="I28" s="26" t="s">
-        <v>708</v>
+        <v>271</v>
       </c>
       <c r="J28" s="38"/>
       <c r="K28" s="38"/>
@@ -21540,13 +21537,13 @@
         <v>44</v>
       </c>
       <c r="B29" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C29" s="39">
         <v>28.0</v>
       </c>
       <c r="D29" s="39" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E29" s="39" t="s">
         <v>258</v>
@@ -21598,13 +21595,13 @@
         <v>44</v>
       </c>
       <c r="B30" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C30" s="38">
         <v>29.0</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E30" s="38" t="s">
         <v>258</v>
@@ -21617,7 +21614,7 @@
         <v>270</v>
       </c>
       <c r="I30" s="26" t="s">
-        <v>708</v>
+        <v>271</v>
       </c>
       <c r="J30" s="38"/>
       <c r="K30" s="38"/>
@@ -21658,13 +21655,13 @@
         <v>44</v>
       </c>
       <c r="B31" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C31" s="39">
         <v>30.0</v>
       </c>
       <c r="D31" s="39" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E31" s="39" t="s">
         <v>258</v>
@@ -21677,7 +21674,7 @@
         <v>270</v>
       </c>
       <c r="I31" s="30" t="s">
-        <v>708</v>
+        <v>271</v>
       </c>
       <c r="J31" s="39"/>
       <c r="K31" s="39"/>
@@ -21718,13 +21715,13 @@
         <v>44</v>
       </c>
       <c r="B32" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C32" s="38">
         <v>31.0</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E32" s="38" t="s">
         <v>258</v>
@@ -21776,13 +21773,13 @@
         <v>44</v>
       </c>
       <c r="B33" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C33" s="39">
         <v>32.0</v>
       </c>
       <c r="D33" s="39" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E33" s="39" t="s">
         <v>258</v>
@@ -21834,13 +21831,13 @@
         <v>44</v>
       </c>
       <c r="B34" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C34" s="38">
         <v>33.0</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E34" s="38" t="s">
         <v>258</v>
@@ -21892,13 +21889,13 @@
         <v>44</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C35" s="39">
         <v>34.0</v>
       </c>
       <c r="D35" s="39" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E35" s="39" t="s">
         <v>258</v>
@@ -21950,13 +21947,13 @@
         <v>44</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C36" s="38">
         <v>35.0</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E36" s="38" t="s">
         <v>258</v>
@@ -22008,13 +22005,13 @@
         <v>44</v>
       </c>
       <c r="B37" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C37" s="39">
         <v>36.0</v>
       </c>
       <c r="D37" s="39" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E37" s="39" t="s">
         <v>258</v>
@@ -22066,13 +22063,13 @@
         <v>44</v>
       </c>
       <c r="B38" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C38" s="38">
         <v>37.0</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E38" s="38" t="s">
         <v>504</v>
@@ -22126,13 +22123,13 @@
         <v>44</v>
       </c>
       <c r="B39" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C39" s="39">
         <v>38.0</v>
       </c>
       <c r="D39" s="39" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E39" s="39" t="s">
         <v>258</v>
@@ -22184,13 +22181,13 @@
         <v>44</v>
       </c>
       <c r="B40" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C40" s="38">
         <v>39.0</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E40" s="38" t="s">
         <v>258</v>
@@ -22244,13 +22241,13 @@
         <v>44</v>
       </c>
       <c r="B41" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C41" s="39">
         <v>40.0</v>
       </c>
       <c r="D41" s="39" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E41" s="39" t="s">
         <v>258</v>
@@ -22304,13 +22301,13 @@
         <v>44</v>
       </c>
       <c r="B42" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C42" s="38">
         <v>41.0</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E42" s="38" t="s">
         <v>258</v>
@@ -22362,13 +22359,13 @@
         <v>44</v>
       </c>
       <c r="B43" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C43" s="39">
         <v>42.0</v>
       </c>
       <c r="D43" s="39" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E43" s="39" t="s">
         <v>258</v>
@@ -22422,13 +22419,13 @@
         <v>44</v>
       </c>
       <c r="B44" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C44" s="38">
         <v>43.0</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E44" s="38" t="s">
         <v>258</v>
@@ -22482,13 +22479,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C45" s="39">
         <v>44.0</v>
       </c>
       <c r="D45" s="39" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E45" s="39" t="s">
         <v>258</v>
@@ -22540,13 +22537,13 @@
         <v>44</v>
       </c>
       <c r="B46" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C46" s="38">
         <v>45.0</v>
       </c>
       <c r="D46" s="38" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="E46" s="38" t="s">
         <v>285</v>
@@ -22555,7 +22552,7 @@
         <v>280</v>
       </c>
       <c r="G46" s="38" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="H46" s="38" t="s">
         <v>439</v>
@@ -22602,13 +22599,13 @@
         <v>44</v>
       </c>
       <c r="B47" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C47" s="39">
         <v>46.0</v>
       </c>
       <c r="D47" s="39" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="E47" s="39" t="s">
         <v>285</v>
@@ -22617,7 +22614,7 @@
         <v>280</v>
       </c>
       <c r="G47" s="39" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="H47" s="39" t="s">
         <v>439</v>
@@ -22664,13 +22661,13 @@
         <v>44</v>
       </c>
       <c r="B48" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C48" s="38">
         <v>47.0</v>
       </c>
       <c r="D48" s="38" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="E48" s="38" t="s">
         <v>285</v>
@@ -22679,7 +22676,7 @@
         <v>280</v>
       </c>
       <c r="G48" s="38" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="H48" s="38" t="s">
         <v>439</v>
@@ -22726,13 +22723,13 @@
         <v>44</v>
       </c>
       <c r="B49" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C49" s="39">
         <v>48.0</v>
       </c>
       <c r="D49" s="39" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E49" s="39" t="s">
         <v>285</v>
@@ -22741,7 +22738,7 @@
         <v>280</v>
       </c>
       <c r="G49" s="39" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="H49" s="39" t="s">
         <v>439</v>
@@ -22788,13 +22785,13 @@
         <v>44</v>
       </c>
       <c r="B50" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C50" s="38">
         <v>49.0</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="E50" s="38" t="s">
         <v>285</v>
@@ -22803,7 +22800,7 @@
         <v>280</v>
       </c>
       <c r="G50" s="38" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="H50" s="38" t="s">
         <v>439</v>
@@ -22850,13 +22847,13 @@
         <v>44</v>
       </c>
       <c r="B51" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C51" s="39">
         <v>50.0</v>
       </c>
       <c r="D51" s="39" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E51" s="39" t="s">
         <v>285</v>
@@ -22865,7 +22862,7 @@
         <v>280</v>
       </c>
       <c r="G51" s="39" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="H51" s="39" t="s">
         <v>439</v>
@@ -22912,13 +22909,13 @@
         <v>44</v>
       </c>
       <c r="B52" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C52" s="38">
         <v>51.0</v>
       </c>
       <c r="D52" s="38" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E52" s="38" t="s">
         <v>285</v>
@@ -22927,7 +22924,7 @@
         <v>280</v>
       </c>
       <c r="G52" s="38" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="H52" s="38" t="s">
         <v>439</v>
@@ -22974,13 +22971,13 @@
         <v>44</v>
       </c>
       <c r="B53" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C53" s="39">
         <v>52.0</v>
       </c>
       <c r="D53" s="39" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="E53" s="39" t="s">
         <v>285</v>
@@ -22989,7 +22986,7 @@
         <v>280</v>
       </c>
       <c r="G53" s="39" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="H53" s="39" t="s">
         <v>439</v>
@@ -23036,13 +23033,13 @@
         <v>44</v>
       </c>
       <c r="B54" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C54" s="38">
         <v>53.0</v>
       </c>
       <c r="D54" s="38" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E54" s="38" t="s">
         <v>285</v>
@@ -23051,7 +23048,7 @@
         <v>280</v>
       </c>
       <c r="G54" s="38" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="H54" s="38" t="s">
         <v>439</v>
@@ -23098,13 +23095,13 @@
         <v>44</v>
       </c>
       <c r="B55" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C55" s="39">
         <v>54.0</v>
       </c>
       <c r="D55" s="39" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="E55" s="39" t="s">
         <v>285</v>
@@ -23113,7 +23110,7 @@
         <v>280</v>
       </c>
       <c r="G55" s="39" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="H55" s="39" t="s">
         <v>439</v>
@@ -23160,13 +23157,13 @@
         <v>44</v>
       </c>
       <c r="B56" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C56" s="38">
         <v>55.0</v>
       </c>
       <c r="D56" s="38" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="E56" s="38" t="s">
         <v>285</v>
@@ -23175,7 +23172,7 @@
         <v>280</v>
       </c>
       <c r="G56" s="38" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="H56" s="38" t="s">
         <v>439</v>
@@ -23222,13 +23219,13 @@
         <v>44</v>
       </c>
       <c r="B57" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C57" s="39">
         <v>56.0</v>
       </c>
       <c r="D57" s="39" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="E57" s="39" t="s">
         <v>285</v>
@@ -23237,7 +23234,7 @@
         <v>280</v>
       </c>
       <c r="G57" s="39" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="H57" s="39" t="s">
         <v>439</v>
@@ -23284,13 +23281,13 @@
         <v>44</v>
       </c>
       <c r="B58" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C58" s="38">
         <v>57.0</v>
       </c>
       <c r="D58" s="38" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="E58" s="38" t="s">
         <v>258</v>
@@ -23303,7 +23300,7 @@
         <v>270</v>
       </c>
       <c r="I58" s="26" t="s">
-        <v>708</v>
+        <v>271</v>
       </c>
       <c r="J58" s="38"/>
       <c r="K58" s="38"/>
@@ -23344,7 +23341,7 @@
         <v>44</v>
       </c>
       <c r="B59" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C59" s="39">
         <v>58.0</v>
@@ -23404,7 +23401,7 @@
         <v>44</v>
       </c>
       <c r="B60" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C60" s="38">
         <v>59.0</v>
@@ -23464,13 +23461,13 @@
         <v>44</v>
       </c>
       <c r="B61" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C61" s="39">
         <v>60.0</v>
       </c>
       <c r="D61" s="39" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E61" s="39" t="s">
         <v>258</v>
@@ -23524,13 +23521,13 @@
         <v>44</v>
       </c>
       <c r="B62" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C62" s="38">
         <v>61.0</v>
       </c>
       <c r="D62" s="38" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="E62" s="38" t="s">
         <v>258</v>
@@ -23564,13 +23561,13 @@
         <v>44</v>
       </c>
       <c r="B63" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C63" s="39">
         <v>62.0</v>
       </c>
       <c r="D63" s="39" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="E63" s="39" t="s">
         <v>258</v>
@@ -23624,13 +23621,13 @@
         <v>44</v>
       </c>
       <c r="B64" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C64" s="38">
         <v>63.0</v>
       </c>
       <c r="D64" s="38" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E64" s="38" t="s">
         <v>258</v>
@@ -23667,13 +23664,13 @@
         <v>44</v>
       </c>
       <c r="B65" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C65" s="39">
         <v>64.0</v>
       </c>
       <c r="D65" s="39" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E65" s="39" t="s">
         <v>258</v>
@@ -23727,13 +23724,13 @@
         <v>44</v>
       </c>
       <c r="B66" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C66" s="38">
         <v>65.0</v>
       </c>
       <c r="D66" s="38" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E66" s="38" t="s">
         <v>258</v>
@@ -23765,13 +23762,13 @@
         <v>44</v>
       </c>
       <c r="B67" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C67" s="39">
         <v>66.0</v>
       </c>
       <c r="D67" s="39" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="E67" s="39" t="s">
         <v>258</v>
@@ -23823,13 +23820,13 @@
         <v>44</v>
       </c>
       <c r="B68" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C68" s="38">
         <v>67.0</v>
       </c>
       <c r="D68" s="26" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="E68" s="38" t="s">
         <v>258</v>
@@ -23867,13 +23864,13 @@
         <v>44</v>
       </c>
       <c r="B69" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C69" s="39">
         <v>68.0</v>
       </c>
       <c r="D69" s="30" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="E69" s="39" t="s">
         <v>258</v>
@@ -23911,13 +23908,13 @@
         <v>44</v>
       </c>
       <c r="B70" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C70" s="38">
         <v>69.0</v>
       </c>
       <c r="D70" s="26" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="E70" s="38" t="s">
         <v>258</v>
@@ -23955,13 +23952,13 @@
         <v>44</v>
       </c>
       <c r="B71" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C71" s="39">
         <v>70.0</v>
       </c>
       <c r="D71" s="30" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E71" s="30" t="s">
         <v>428</v>
@@ -23999,13 +23996,13 @@
         <v>44</v>
       </c>
       <c r="B72" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C72" s="38">
         <v>71.0</v>
       </c>
       <c r="D72" s="26" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E72" s="38" t="s">
         <v>258</v>
@@ -24043,13 +24040,13 @@
         <v>44</v>
       </c>
       <c r="B73" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C73" s="39">
         <v>72.0</v>
       </c>
       <c r="D73" s="30" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E73" s="39" t="s">
         <v>258</v>
@@ -24087,13 +24084,13 @@
         <v>44</v>
       </c>
       <c r="B74" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C74" s="38">
         <v>73.0</v>
       </c>
       <c r="D74" s="26" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E74" s="26" t="s">
         <v>428</v>
@@ -24131,13 +24128,13 @@
         <v>44</v>
       </c>
       <c r="B75" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C75" s="39">
         <v>74.0</v>
       </c>
       <c r="D75" s="30" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E75" s="39" t="s">
         <v>258</v>
@@ -24175,13 +24172,13 @@
         <v>44</v>
       </c>
       <c r="B76" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C76" s="38">
         <v>75.0</v>
       </c>
       <c r="D76" s="26" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="E76" s="38" t="s">
         <v>258</v>
@@ -24219,13 +24216,13 @@
         <v>44</v>
       </c>
       <c r="B77" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C77" s="39">
         <v>76.0</v>
       </c>
       <c r="D77" s="39" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E77" s="39" t="s">
         <v>258</v>
@@ -24277,13 +24274,13 @@
         <v>44</v>
       </c>
       <c r="B78" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C78" s="38">
         <v>77.0</v>
       </c>
       <c r="D78" s="38" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="E78" s="38" t="s">
         <v>258</v>
@@ -24335,13 +24332,13 @@
         <v>44</v>
       </c>
       <c r="B79" s="39" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C79" s="39">
         <v>78.0</v>
       </c>
       <c r="D79" s="39" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E79" s="39" t="s">
         <v>258</v>
@@ -24395,13 +24392,13 @@
         <v>44</v>
       </c>
       <c r="B80" s="38" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C80" s="38">
         <v>79.0</v>
       </c>
       <c r="D80" s="38" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E80" s="38" t="s">
         <v>258</v>
@@ -24414,7 +24411,7 @@
         <v>270</v>
       </c>
       <c r="I80" s="26" t="s">
-        <v>708</v>
+        <v>271</v>
       </c>
       <c r="J80" s="38"/>
       <c r="K80" s="38"/>
@@ -24545,13 +24542,13 @@
         <v>47</v>
       </c>
       <c r="B2" s="38" t="s">
+        <v>789</v>
+      </c>
+      <c r="C2" s="38">
+        <v>1.0</v>
+      </c>
+      <c r="D2" s="38" t="s">
         <v>790</v>
-      </c>
-      <c r="C2" s="38">
-        <v>1.0</v>
-      </c>
-      <c r="D2" s="38" t="s">
-        <v>791</v>
       </c>
       <c r="E2" s="38" t="s">
         <v>285</v>
@@ -24591,13 +24588,13 @@
         <v>47</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C3" s="39">
         <v>2.0</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="E3" s="39" t="s">
         <v>285</v>
@@ -24637,7 +24634,7 @@
         <v>47</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C4" s="38">
         <v>3.0</v>
@@ -24683,13 +24680,13 @@
         <v>47</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C5" s="39">
         <v>4.0</v>
       </c>
       <c r="D5" s="39" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E5" s="39" t="s">
         <v>285</v>
@@ -24729,13 +24726,13 @@
         <v>47</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C6" s="38">
         <v>5.0</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E6" s="38" t="s">
         <v>285</v>
@@ -24775,7 +24772,7 @@
         <v>47</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C7" s="39">
         <v>6.0</v>
@@ -24821,7 +24818,7 @@
         <v>47</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C8" s="38">
         <v>7.0</v>
@@ -24857,7 +24854,7 @@
         <v>47</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C9" s="39">
         <v>8.0</v>
@@ -24899,7 +24896,7 @@
         <v>47</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C10" s="38">
         <v>9.0</v>
@@ -24943,7 +24940,7 @@
         <v>47</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C11" s="39">
         <v>10.0</v>
@@ -24985,7 +24982,7 @@
         <v>47</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C12" s="38">
         <v>11.0</v>
@@ -25023,7 +25020,7 @@
         <v>47</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C13" s="39">
         <v>12.0</v>
@@ -25067,7 +25064,7 @@
         <v>47</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C14" s="38">
         <v>13.0</v>
@@ -25109,7 +25106,7 @@
         <v>47</v>
       </c>
       <c r="B15" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C15" s="39">
         <v>14.0</v>
@@ -25153,7 +25150,7 @@
         <v>47</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C16" s="38">
         <v>15.0</v>
@@ -25195,7 +25192,7 @@
         <v>47</v>
       </c>
       <c r="B17" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C17" s="39">
         <v>16.0</v>
@@ -25237,13 +25234,13 @@
         <v>47</v>
       </c>
       <c r="B18" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C18" s="38">
         <v>17.0</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E18" s="38" t="s">
         <v>258</v>
@@ -25275,13 +25272,13 @@
         <v>47</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C19" s="39">
         <v>18.0</v>
       </c>
       <c r="D19" s="39" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E19" s="39" t="s">
         <v>258</v>
@@ -25319,13 +25316,13 @@
         <v>47</v>
       </c>
       <c r="B20" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C20" s="38">
         <v>19.0</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E20" s="38" t="s">
         <v>258</v>
@@ -25363,13 +25360,13 @@
         <v>47</v>
       </c>
       <c r="B21" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C21" s="39">
         <v>20.0</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="E21" s="39" t="s">
         <v>258</v>
@@ -25407,13 +25404,13 @@
         <v>47</v>
       </c>
       <c r="B22" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C22" s="38">
         <v>21.0</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E22" s="38" t="s">
         <v>258</v>
@@ -25449,7 +25446,7 @@
         <v>47</v>
       </c>
       <c r="B23" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C23" s="39">
         <v>22.0</v>
@@ -25485,7 +25482,7 @@
         <v>47</v>
       </c>
       <c r="B24" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C24" s="38">
         <v>23.0</v>
@@ -25519,7 +25516,7 @@
         <v>47</v>
       </c>
       <c r="B25" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C25" s="39">
         <v>24.0</v>
@@ -25561,13 +25558,13 @@
         <v>47</v>
       </c>
       <c r="B26" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C26" s="38">
         <v>25.0</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E26" s="38" t="s">
         <v>258</v>
@@ -25603,13 +25600,13 @@
         <v>47</v>
       </c>
       <c r="B27" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C27" s="39">
         <v>26.0</v>
       </c>
       <c r="D27" s="39" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E27" s="39" t="s">
         <v>258</v>
@@ -25647,13 +25644,13 @@
         <v>47</v>
       </c>
       <c r="B28" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C28" s="38">
         <v>27.0</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E28" s="38" t="s">
         <v>269</v>
@@ -25691,13 +25688,13 @@
         <v>47</v>
       </c>
       <c r="B29" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C29" s="39">
         <v>28.0</v>
       </c>
       <c r="D29" s="39" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E29" s="39" t="s">
         <v>269</v>
@@ -25735,13 +25732,13 @@
         <v>47</v>
       </c>
       <c r="B30" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C30" s="38">
         <v>29.0</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E30" s="38" t="s">
         <v>258</v>
@@ -25777,7 +25774,7 @@
         <v>47</v>
       </c>
       <c r="B31" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C31" s="39">
         <v>30.0</v>
@@ -25819,7 +25816,7 @@
         <v>47</v>
       </c>
       <c r="B32" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C32" s="38">
         <v>31.0</v>
@@ -25863,13 +25860,13 @@
         <v>47</v>
       </c>
       <c r="B33" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C33" s="39">
         <v>32.0</v>
       </c>
       <c r="D33" s="39" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E33" s="39" t="s">
         <v>258</v>
@@ -25901,13 +25898,13 @@
         <v>47</v>
       </c>
       <c r="B34" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C34" s="38">
         <v>33.0</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E34" s="38" t="s">
         <v>258</v>
@@ -25945,13 +25942,13 @@
         <v>47</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C35" s="39">
         <v>34.0</v>
       </c>
       <c r="D35" s="39" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E35" s="39" t="s">
         <v>258</v>
@@ -25989,13 +25986,13 @@
         <v>47</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C36" s="38">
         <v>35.0</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E36" s="38" t="s">
         <v>504</v>
@@ -26033,13 +26030,13 @@
         <v>47</v>
       </c>
       <c r="B37" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C37" s="39">
         <v>36.0</v>
       </c>
       <c r="D37" s="39" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E37" s="39" t="s">
         <v>258</v>
@@ -26077,13 +26074,13 @@
         <v>47</v>
       </c>
       <c r="B38" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C38" s="38">
         <v>37.0</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E38" s="38" t="s">
         <v>258</v>
@@ -26121,13 +26118,13 @@
         <v>47</v>
       </c>
       <c r="B39" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C39" s="39">
         <v>38.0</v>
       </c>
       <c r="D39" s="39" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E39" s="39" t="s">
         <v>258</v>
@@ -26155,13 +26152,13 @@
         <v>47</v>
       </c>
       <c r="B40" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C40" s="38">
         <v>39.0</v>
       </c>
       <c r="D40" s="26" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E40" s="38" t="s">
         <v>504</v>
@@ -26199,13 +26196,13 @@
         <v>47</v>
       </c>
       <c r="B41" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C41" s="39">
         <v>40.0</v>
       </c>
       <c r="D41" s="30" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E41" s="39" t="s">
         <v>258</v>
@@ -26241,13 +26238,13 @@
         <v>47</v>
       </c>
       <c r="B42" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C42" s="38">
         <v>41.0</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E42" s="38" t="s">
         <v>258</v>
@@ -26285,13 +26282,13 @@
         <v>47</v>
       </c>
       <c r="B43" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C43" s="39">
         <v>42.0</v>
       </c>
       <c r="D43" s="30" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E43" s="39" t="s">
         <v>258</v>
@@ -26329,13 +26326,13 @@
         <v>47</v>
       </c>
       <c r="B44" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C44" s="38">
         <v>43.0</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E44" s="38" t="s">
         <v>258</v>
@@ -26363,7 +26360,7 @@
         <v>47</v>
       </c>
       <c r="B45" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C45" s="39">
         <v>44.0</v>
@@ -26407,7 +26404,7 @@
         <v>47</v>
       </c>
       <c r="B46" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C46" s="38">
         <v>45.0</v>
@@ -26451,7 +26448,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C47" s="39">
         <v>46.0</v>
@@ -26495,7 +26492,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C48" s="38">
         <v>47.0</v>
@@ -26539,7 +26536,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C49" s="39">
         <v>48.0</v>
@@ -26583,13 +26580,13 @@
         <v>47</v>
       </c>
       <c r="B50" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C50" s="38">
         <v>49.0</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E50" s="38" t="s">
         <v>258</v>
@@ -26627,13 +26624,13 @@
         <v>47</v>
       </c>
       <c r="B51" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C51" s="39">
         <v>50.0</v>
       </c>
       <c r="D51" s="39" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E51" s="39" t="s">
         <v>258</v>
@@ -26663,13 +26660,13 @@
         <v>47</v>
       </c>
       <c r="B52" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C52" s="38">
         <v>51.0</v>
       </c>
       <c r="D52" s="38" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="E52" s="38" t="s">
         <v>258</v>
@@ -26699,13 +26696,13 @@
         <v>47</v>
       </c>
       <c r="B53" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C53" s="39">
         <v>52.0</v>
       </c>
       <c r="D53" s="39" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E53" s="39" t="s">
         <v>258</v>
@@ -26735,13 +26732,13 @@
         <v>47</v>
       </c>
       <c r="B54" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C54" s="38">
         <v>53.0</v>
       </c>
       <c r="D54" s="38" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="E54" s="38" t="s">
         <v>258</v>
@@ -26771,13 +26768,13 @@
         <v>47</v>
       </c>
       <c r="B55" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C55" s="39">
         <v>54.0</v>
       </c>
       <c r="D55" s="39" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E55" s="39" t="s">
         <v>258</v>
@@ -26807,13 +26804,13 @@
         <v>47</v>
       </c>
       <c r="B56" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C56" s="38">
         <v>55.0</v>
       </c>
       <c r="D56" s="38" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E56" s="38" t="s">
         <v>258</v>
@@ -26843,7 +26840,7 @@
         <v>47</v>
       </c>
       <c r="B57" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C57" s="39">
         <v>56.0</v>
@@ -26887,7 +26884,7 @@
         <v>47</v>
       </c>
       <c r="B58" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C58" s="38">
         <v>57.0</v>
@@ -26931,7 +26928,7 @@
         <v>47</v>
       </c>
       <c r="B59" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C59" s="39">
         <v>58.0</v>
@@ -26975,7 +26972,7 @@
         <v>47</v>
       </c>
       <c r="B60" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C60" s="38">
         <v>59.0</v>
@@ -27019,7 +27016,7 @@
         <v>47</v>
       </c>
       <c r="B61" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C61" s="39">
         <v>60.0</v>
@@ -27057,13 +27054,13 @@
         <v>47</v>
       </c>
       <c r="B62" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C62" s="38">
         <v>61.0</v>
       </c>
       <c r="D62" s="38" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E62" s="38" t="s">
         <v>258</v>
@@ -27101,13 +27098,13 @@
         <v>47</v>
       </c>
       <c r="B63" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C63" s="39">
         <v>62.0</v>
       </c>
       <c r="D63" s="39" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E63" s="39" t="s">
         <v>258</v>
@@ -27137,7 +27134,7 @@
         <v>47</v>
       </c>
       <c r="B64" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C64" s="38">
         <v>63.0</v>
@@ -27173,13 +27170,13 @@
         <v>47</v>
       </c>
       <c r="B65" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C65" s="39">
         <v>64.0</v>
       </c>
       <c r="D65" s="30" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="E65" s="39" t="s">
         <v>258</v>
@@ -27209,7 +27206,7 @@
         <v>47</v>
       </c>
       <c r="B66" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C66" s="38">
         <v>65.0</v>
@@ -27253,7 +27250,7 @@
         <v>47</v>
       </c>
       <c r="B67" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C67" s="39">
         <v>66.0</v>
@@ -27289,13 +27286,13 @@
         <v>47</v>
       </c>
       <c r="B68" s="38" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C68" s="38">
         <v>67.0</v>
       </c>
       <c r="D68" s="26" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E68" s="38" t="s">
         <v>258</v>
@@ -27325,13 +27322,13 @@
         <v>47</v>
       </c>
       <c r="B69" s="39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C69" s="39">
         <v>68.0</v>
       </c>
       <c r="D69" s="30" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E69" s="30" t="s">
         <v>285</v>
@@ -27433,13 +27430,13 @@
         <v>296</v>
       </c>
       <c r="M1" s="45" t="s">
+        <v>819</v>
+      </c>
+      <c r="N1" s="45" t="s">
         <v>820</v>
       </c>
-      <c r="N1" s="45" t="s">
+      <c r="O1" s="45" t="s">
         <v>821</v>
-      </c>
-      <c r="O1" s="45" t="s">
-        <v>822</v>
       </c>
       <c r="P1" s="45" t="s">
         <v>433</v>
@@ -27462,7 +27459,7 @@
         <v>1.0</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="E2" s="38" t="s">
         <v>285</v>
@@ -27514,7 +27511,7 @@
         <v>2.0</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="E3" s="39" t="s">
         <v>285</v>
@@ -27618,7 +27615,7 @@
         <v>4.0</v>
       </c>
       <c r="D5" s="39" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E5" s="39" t="s">
         <v>285</v>
@@ -27670,7 +27667,7 @@
         <v>5.0</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E6" s="38" t="s">
         <v>285</v>
@@ -28254,7 +28251,7 @@
         <v>17.0</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E18" s="38" t="s">
         <v>258</v>
@@ -28306,7 +28303,7 @@
         <v>18.0</v>
       </c>
       <c r="D19" s="39" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E19" s="39" t="s">
         <v>258</v>
@@ -28358,7 +28355,7 @@
         <v>19.0</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E20" s="38" t="s">
         <v>258</v>
@@ -28410,7 +28407,7 @@
         <v>20.0</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="E21" s="39" t="s">
         <v>258</v>
@@ -28462,7 +28459,7 @@
         <v>21.0</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E22" s="38" t="s">
         <v>258</v>
@@ -28650,7 +28647,7 @@
         <v>25.0</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E26" s="38" t="s">
         <v>258</v>
@@ -28688,7 +28685,7 @@
         <v>26.0</v>
       </c>
       <c r="D27" s="39" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E27" s="39" t="s">
         <v>258</v>
@@ -28788,7 +28785,7 @@
         <v>28.0</v>
       </c>
       <c r="D29" s="39" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="E29" s="39" t="s">
         <v>258</v>
@@ -28838,7 +28835,7 @@
         <v>29.0</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E30" s="38" t="s">
         <v>258</v>
@@ -28888,7 +28885,7 @@
         <v>30.0</v>
       </c>
       <c r="D31" s="39" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="E31" s="39" t="s">
         <v>258</v>
@@ -28938,7 +28935,7 @@
         <v>31.0</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="E32" s="38" t="s">
         <v>504</v>
@@ -28988,7 +28985,7 @@
         <v>32.0</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="E33" s="39" t="s">
         <v>258</v>
@@ -29038,7 +29035,7 @@
         <v>33.0</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="E34" s="38" t="s">
         <v>258</v>
@@ -29088,7 +29085,7 @@
         <v>34.0</v>
       </c>
       <c r="D35" s="39" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="E35" s="39" t="s">
         <v>258</v>
@@ -29134,7 +29131,7 @@
         <v>35.0</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E36" s="38" t="s">
         <v>504</v>
@@ -29184,7 +29181,7 @@
         <v>36.0</v>
       </c>
       <c r="D37" s="39" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E37" s="39" t="s">
         <v>258</v>
@@ -29232,7 +29229,7 @@
         <v>37.0</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E38" s="38" t="s">
         <v>258</v>
@@ -29282,7 +29279,7 @@
         <v>38.0</v>
       </c>
       <c r="D39" s="39" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E39" s="39" t="s">
         <v>258</v>
@@ -29332,7 +29329,7 @@
         <v>39.0</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E40" s="38" t="s">
         <v>258</v>
@@ -29630,7 +29627,7 @@
         <v>45.0</v>
       </c>
       <c r="D46" s="38" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E46" s="38" t="s">
         <v>258</v>
@@ -29680,7 +29677,7 @@
         <v>46.0</v>
       </c>
       <c r="D47" s="39" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E47" s="39" t="s">
         <v>258</v>
@@ -29718,7 +29715,7 @@
         <v>47.0</v>
       </c>
       <c r="D48" s="38" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="E48" s="38" t="s">
         <v>258</v>
@@ -29756,7 +29753,7 @@
         <v>48.0</v>
       </c>
       <c r="D49" s="39" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E49" s="39" t="s">
         <v>258</v>
@@ -29794,7 +29791,7 @@
         <v>49.0</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="E50" s="38" t="s">
         <v>258</v>
@@ -29832,7 +29829,7 @@
         <v>50.0</v>
       </c>
       <c r="D51" s="39" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E51" s="39" t="s">
         <v>258</v>
@@ -29870,7 +29867,7 @@
         <v>51.0</v>
       </c>
       <c r="D52" s="38" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E52" s="38" t="s">
         <v>258</v>
@@ -30158,7 +30155,7 @@
         <v>57.0</v>
       </c>
       <c r="D58" s="38" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E58" s="38" t="s">
         <v>258</v>
@@ -30208,7 +30205,7 @@
         <v>58.0</v>
       </c>
       <c r="D59" s="39" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E59" s="39" t="s">
         <v>258</v>
@@ -30256,7 +30253,7 @@
         <v>59.0</v>
       </c>
       <c r="D60" s="38" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E60" s="38" t="s">
         <v>269</v>
@@ -30342,7 +30339,7 @@
         <v>61.0</v>
       </c>
       <c r="D62" s="26" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="E62" s="38" t="s">
         <v>269</v>
@@ -30392,7 +30389,7 @@
         <v>62.0</v>
       </c>
       <c r="D63" s="39" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E63" s="39" t="s">
         <v>258</v>
@@ -30428,7 +30425,7 @@
         <v>63.0</v>
       </c>
       <c r="D64" s="38" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="E64" s="38" t="s">
         <v>285</v>
@@ -30437,7 +30434,7 @@
         <v>280</v>
       </c>
       <c r="G64" s="25" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="H64" s="26" t="s">
         <v>439</v>
@@ -30480,7 +30477,7 @@
         <v>64.0</v>
       </c>
       <c r="D65" s="30" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="E65" s="30" t="s">
         <v>504</v>
@@ -30528,7 +30525,7 @@
         <v>65.0</v>
       </c>
       <c r="D66" s="26" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="E66" s="38" t="s">
         <v>258</v>
@@ -30574,7 +30571,7 @@
         <v>66.0</v>
       </c>
       <c r="D67" s="30" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="E67" s="39" t="s">
         <v>258</v>
@@ -30620,7 +30617,7 @@
         <v>67.0</v>
       </c>
       <c r="D68" s="26" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="E68" s="38" t="s">
         <v>269</v>
@@ -30668,7 +30665,7 @@
         <v>68.0</v>
       </c>
       <c r="D69" s="39" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E69" s="39" t="s">
         <v>285</v>
@@ -30677,7 +30674,7 @@
         <v>280</v>
       </c>
       <c r="G69" s="29" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="H69" s="30" t="s">
         <v>439</v>
@@ -30720,7 +30717,7 @@
         <v>69.0</v>
       </c>
       <c r="D70" s="38" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="E70" s="38" t="s">
         <v>258</v>
@@ -30756,7 +30753,7 @@
         <v>70.0</v>
       </c>
       <c r="D71" s="39" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="E71" s="39" t="s">
         <v>269</v>
@@ -30794,7 +30791,7 @@
         <v>71.0</v>
       </c>
       <c r="D72" s="38" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="E72" s="38" t="s">
         <v>285</v>
@@ -30803,7 +30800,7 @@
         <v>280</v>
       </c>
       <c r="G72" s="25" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="H72" s="26" t="s">
         <v>439</v>
@@ -30846,7 +30843,7 @@
         <v>72.0</v>
       </c>
       <c r="D73" s="39" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="E73" s="39" t="s">
         <v>285</v>
@@ -30855,7 +30852,7 @@
         <v>280</v>
       </c>
       <c r="G73" s="29" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="H73" s="30" t="s">
         <v>439</v>
@@ -30898,7 +30895,7 @@
         <v>73.0</v>
       </c>
       <c r="D74" s="38" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="E74" s="38" t="s">
         <v>258</v>
@@ -30934,7 +30931,7 @@
         <v>74.0</v>
       </c>
       <c r="D75" s="39" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="E75" s="39" t="s">
         <v>269</v>
@@ -31062,13 +31059,13 @@
         <v>32</v>
       </c>
       <c r="B2" s="38" t="s">
+        <v>844</v>
+      </c>
+      <c r="C2" s="38">
+        <v>1.0</v>
+      </c>
+      <c r="D2" s="26" t="s">
         <v>845</v>
-      </c>
-      <c r="C2" s="38">
-        <v>1.0</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>846</v>
       </c>
       <c r="E2" s="38" t="s">
         <v>285</v>
@@ -31108,7 +31105,7 @@
         <v>32</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C3" s="39">
         <v>2.0</v>
@@ -31154,7 +31151,7 @@
         <v>32</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C4" s="38">
         <v>3.0</v>
@@ -31200,7 +31197,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C5" s="39">
         <v>4.0</v>
@@ -31246,7 +31243,7 @@
         <v>32</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C6" s="38">
         <v>5.0</v>
@@ -31292,13 +31289,13 @@
         <v>32</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C7" s="39">
         <v>6.0</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="E7" s="39" t="s">
         <v>285</v>
@@ -31338,13 +31335,13 @@
         <v>32</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C8" s="38">
         <v>7.0</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="E8" s="38" t="s">
         <v>285</v>
@@ -31384,13 +31381,13 @@
         <v>32</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C9" s="39">
         <v>8.0</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="E9" s="39" t="s">
         <v>285</v>
@@ -31430,7 +31427,7 @@
         <v>32</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C10" s="38">
         <v>9.0</v>
@@ -31476,7 +31473,7 @@
         <v>32</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C11" s="39">
         <v>10.0</v>
@@ -31522,13 +31519,13 @@
         <v>32</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C12" s="38">
         <v>11.0</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E12" s="38" t="s">
         <v>285</v>
@@ -31568,13 +31565,13 @@
         <v>32</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C13" s="39">
         <v>12.0</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="E13" s="39" t="s">
         <v>285</v>
@@ -31614,7 +31611,7 @@
         <v>32</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C14" s="38">
         <v>13.0</v>
@@ -31660,13 +31657,13 @@
         <v>32</v>
       </c>
       <c r="B15" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C15" s="39">
         <v>14.0</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="E15" s="39" t="s">
         <v>258</v>
@@ -31692,7 +31689,7 @@
         <v>32</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C16" s="38">
         <v>15.0</v>
@@ -31734,7 +31731,7 @@
         <v>32</v>
       </c>
       <c r="B17" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C17" s="39">
         <v>16.0</v>
@@ -31778,7 +31775,7 @@
         <v>32</v>
       </c>
       <c r="B18" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C18" s="38">
         <v>17.0</v>
@@ -31820,7 +31817,7 @@
         <v>32</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C19" s="39">
         <v>18.0</v>
@@ -31864,7 +31861,7 @@
         <v>32</v>
       </c>
       <c r="B20" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C20" s="38">
         <v>19.0</v>
@@ -31908,7 +31905,7 @@
         <v>32</v>
       </c>
       <c r="B21" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C21" s="39">
         <v>20.0</v>
@@ -31950,13 +31947,13 @@
         <v>32</v>
       </c>
       <c r="B22" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C22" s="38">
         <v>21.0</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="E22" s="38" t="s">
         <v>258</v>
@@ -31994,7 +31991,7 @@
         <v>32</v>
       </c>
       <c r="B23" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C23" s="39">
         <v>22.0</v>
@@ -32036,7 +32033,7 @@
         <v>32</v>
       </c>
       <c r="B24" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C24" s="38">
         <v>23.0</v>
@@ -32080,7 +32077,7 @@
         <v>32</v>
       </c>
       <c r="B25" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C25" s="39">
         <v>24.0</v>
@@ -32122,7 +32119,7 @@
         <v>32</v>
       </c>
       <c r="B26" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C26" s="38">
         <v>25.0</v>
@@ -32164,7 +32161,7 @@
         <v>32</v>
       </c>
       <c r="B27" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C27" s="39">
         <v>26.0</v>
@@ -32208,7 +32205,7 @@
         <v>32</v>
       </c>
       <c r="B28" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C28" s="38">
         <v>27.0</v>
@@ -32252,13 +32249,13 @@
         <v>32</v>
       </c>
       <c r="B29" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C29" s="39">
         <v>28.0</v>
       </c>
       <c r="D29" s="39" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E29" s="39" t="s">
         <v>258</v>
@@ -32296,7 +32293,7 @@
         <v>32</v>
       </c>
       <c r="B30" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C30" s="38">
         <v>29.0</v>
@@ -32340,7 +32337,7 @@
         <v>32</v>
       </c>
       <c r="B31" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C31" s="39">
         <v>30.0</v>
@@ -32384,7 +32381,7 @@
         <v>32</v>
       </c>
       <c r="B32" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C32" s="38">
         <v>31.0</v>
@@ -32428,7 +32425,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C33" s="39">
         <v>32.0</v>
@@ -32472,7 +32469,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C34" s="38">
         <v>33.0</v>
@@ -32516,13 +32513,13 @@
         <v>32</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C35" s="39">
         <v>34.0</v>
       </c>
       <c r="D35" s="39" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="E35" s="39" t="s">
         <v>258</v>
@@ -32551,13 +32548,13 @@
         <v>32</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C36" s="38">
         <v>35.0</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E36" s="38" t="s">
         <v>258</v>
@@ -32586,7 +32583,7 @@
         <v>32</v>
       </c>
       <c r="B37" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C37" s="39">
         <v>36.0</v>
@@ -32621,7 +32618,7 @@
         <v>32</v>
       </c>
       <c r="B38" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C38" s="38">
         <v>37.0</v>
@@ -32657,13 +32654,13 @@
         <v>32</v>
       </c>
       <c r="B39" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C39" s="39">
         <v>38.0</v>
       </c>
       <c r="D39" s="39" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="E39" s="39" t="s">
         <v>285</v>
@@ -32672,7 +32669,7 @@
         <v>280</v>
       </c>
       <c r="G39" s="39" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="H39" s="30" t="s">
         <v>439</v>
@@ -32703,13 +32700,13 @@
         <v>32</v>
       </c>
       <c r="B40" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C40" s="38">
         <v>39.0</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="E40" s="38" t="s">
         <v>285</v>
@@ -32718,7 +32715,7 @@
         <v>280</v>
       </c>
       <c r="G40" s="38" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="H40" s="26" t="s">
         <v>439</v>
@@ -32749,13 +32746,13 @@
         <v>32</v>
       </c>
       <c r="B41" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C41" s="39">
         <v>40.0</v>
       </c>
       <c r="D41" s="39" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="E41" s="39" t="s">
         <v>258</v>
@@ -32791,7 +32788,7 @@
         <v>32</v>
       </c>
       <c r="B42" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C42" s="38">
         <v>41.0</v>
@@ -32837,7 +32834,7 @@
         <v>32</v>
       </c>
       <c r="B43" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C43" s="39">
         <v>42.0</v>
@@ -32883,7 +32880,7 @@
         <v>32</v>
       </c>
       <c r="B44" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C44" s="38">
         <v>43.0</v>
@@ -32904,7 +32901,7 @@
       <c r="I44" s="38"/>
       <c r="J44" s="38"/>
       <c r="K44" s="26" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="L44" s="38" t="s">
         <v>307</v>
@@ -32918,7 +32915,7 @@
         <v>32</v>
       </c>
       <c r="B45" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C45" s="39">
         <v>44.0</v>
@@ -32933,7 +32930,7 @@
         <v>280</v>
       </c>
       <c r="G45" s="39" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="H45" s="30" t="s">
         <v>439</v>
@@ -32964,7 +32961,7 @@
         <v>32</v>
       </c>
       <c r="B46" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C46" s="38">
         <v>45.0</v>
@@ -32979,7 +32976,7 @@
         <v>280</v>
       </c>
       <c r="G46" s="38" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="H46" s="26" t="s">
         <v>439</v>
@@ -33010,13 +33007,13 @@
         <v>32</v>
       </c>
       <c r="B47" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C47" s="39">
         <v>46.0</v>
       </c>
       <c r="D47" s="39" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="E47" s="39" t="s">
         <v>258</v>
@@ -33031,7 +33028,7 @@
       <c r="I47" s="39"/>
       <c r="J47" s="39"/>
       <c r="K47" s="30" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="L47" s="39" t="s">
         <v>305</v>
@@ -33054,13 +33051,13 @@
         <v>32</v>
       </c>
       <c r="B48" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C48" s="38">
         <v>47.0</v>
       </c>
       <c r="D48" s="38" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="E48" s="38" t="s">
         <v>504</v>
@@ -33098,13 +33095,13 @@
         <v>32</v>
       </c>
       <c r="B49" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C49" s="39">
         <v>48.0</v>
       </c>
       <c r="D49" s="39" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="E49" s="39" t="s">
         <v>258</v>
@@ -33140,13 +33137,13 @@
         <v>32</v>
       </c>
       <c r="B50" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C50" s="38">
         <v>49.0</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="E50" s="38" t="s">
         <v>258</v>
@@ -33184,13 +33181,13 @@
         <v>32</v>
       </c>
       <c r="B51" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C51" s="39">
         <v>50.0</v>
       </c>
       <c r="D51" s="39" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="E51" s="39" t="s">
         <v>258</v>
@@ -33228,13 +33225,13 @@
         <v>32</v>
       </c>
       <c r="B52" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C52" s="38">
         <v>51.0</v>
       </c>
       <c r="D52" s="26" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="E52" s="38" t="s">
         <v>285</v>
@@ -33272,13 +33269,13 @@
         <v>32</v>
       </c>
       <c r="B53" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C53" s="39">
         <v>52.0</v>
       </c>
       <c r="D53" s="39" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="E53" s="39" t="s">
         <v>285</v>
@@ -33316,13 +33313,13 @@
         <v>32</v>
       </c>
       <c r="B54" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C54" s="38">
         <v>53.0</v>
       </c>
       <c r="D54" s="38" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="E54" s="38" t="s">
         <v>285</v>
@@ -33360,13 +33357,13 @@
         <v>32</v>
       </c>
       <c r="B55" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C55" s="39">
         <v>54.0</v>
       </c>
       <c r="D55" s="39" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="E55" s="39" t="s">
         <v>258</v>
@@ -33393,13 +33390,13 @@
         <v>32</v>
       </c>
       <c r="B56" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C56" s="38">
         <v>55.0</v>
       </c>
       <c r="D56" s="38" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="E56" s="38" t="s">
         <v>258</v>
@@ -33414,7 +33411,7 @@
       <c r="I56" s="26"/>
       <c r="J56" s="38"/>
       <c r="K56" s="26" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="L56" s="38" t="s">
         <v>305</v>
@@ -33437,7 +33434,7 @@
         <v>32</v>
       </c>
       <c r="B57" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C57" s="39">
         <v>56.0</v>
@@ -33471,7 +33468,7 @@
         <v>32</v>
       </c>
       <c r="B58" s="38" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C58" s="38">
         <v>57.0</v>
@@ -33505,13 +33502,13 @@
         <v>32</v>
       </c>
       <c r="B59" s="39" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C59" s="39">
         <v>58.0</v>
       </c>
       <c r="D59" s="39" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E59" s="39" t="s">
         <v>258</v>

</xml_diff>